<commit_message>
handled control hazard & bugs fix
</commit_message>
<xml_diff>
--- a/lab5_resource/control.xlsx
+++ b/lab5_resource/control.xlsx
@@ -81,10 +81,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>xx</t>
-  </si>
-  <si>
     <t>Jump</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -436,7 +436,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>11</v>
@@ -635,8 +635,8 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
@@ -664,7 +664,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>xx0x0100x0</v>
+        <v>110x0100x0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>